<commit_message>
documentation + mode numéro 3
</commit_message>
<xml_diff>
--- a/Documentation/PLannification_TPI.xlsx
+++ b/Documentation/PLannification_TPI.xlsx
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM61"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3660,8 +3660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4366,13 +4366,15 @@
       </c>
       <c r="B27" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="7"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="21">
+        <v>0.125</v>
+      </c>
       <c r="H27" s="7"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -4381,7 +4383,7 @@
       <c r="M27" s="43"/>
       <c r="N27" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -4390,13 +4392,15 @@
       </c>
       <c r="B28" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="G28" s="21">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="H28" s="7"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -4405,7 +4409,7 @@
       <c r="M28" s="43"/>
       <c r="N28" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -4650,13 +4654,15 @@
       </c>
       <c r="B39" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="3"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="G39" s="21">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="H39" s="4"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -4665,7 +4671,7 @@
       <c r="M39" s="45"/>
       <c r="N39" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -4921,7 +4927,7 @@
       </c>
       <c r="B50" s="57">
         <f t="shared" si="1"/>
-        <v>6.9444444444444448E-2</v>
+        <v>8.3333333333333343E-2</v>
       </c>
       <c r="C50" s="17">
         <v>2.0833333333333332E-2</v>
@@ -4935,7 +4941,9 @@
       <c r="F50" s="19">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="17">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
@@ -4944,7 +4952,7 @@
       <c r="M50" s="3"/>
       <c r="N50" s="50">
         <f t="shared" si="4"/>
-        <v>6.9444444444444448E-2</v>
+        <v>8.3333333333333343E-2</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -5005,7 +5013,7 @@
       </c>
       <c r="B53" s="57">
         <f t="shared" si="1"/>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="19">
@@ -5017,7 +5025,9 @@
       <c r="F53" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G53" s="3"/>
+      <c r="G53" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -5026,7 +5036,7 @@
       <c r="M53" s="3"/>
       <c r="N53" s="50">
         <f>SUM(C53:M53)</f>
-        <v>0.125</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5062,7 +5072,7 @@
       <c r="A55" s="10"/>
       <c r="B55" s="62">
         <f t="shared" ref="B55:M55" si="5">SUM(B2:B54)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="C55" s="63">
         <f t="shared" si="5"/>
@@ -5082,7 +5092,7 @@
       </c>
       <c r="G55" s="63">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H55" s="63">
         <f t="shared" si="5"/>
@@ -5111,7 +5121,7 @@
       <c r="N55" s="64"/>
       <c r="O55" s="65">
         <f>SUM(N57-N56)</f>
-        <v>2.3333333333333335</v>
+        <v>1.9999999999999998</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5136,7 +5146,7 @@
       </c>
       <c r="N56" s="52">
         <f>SUM(N3:N55)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Ajout et finalisation du monde 3
Début de la sauvegarde
</commit_message>
<xml_diff>
--- a/Documentation/PLannification_TPI.xlsx
+++ b/Documentation/PLannification_TPI.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="70">
   <si>
     <t>Temps nécessaire</t>
   </si>
@@ -223,6 +223,18 @@
   </si>
   <si>
     <t>Mode 1, choisir une entrer et sortie et trouver la solution la plus rapide</t>
+  </si>
+  <si>
+    <t>Afficher chaque trace que l'utilisateur choisi</t>
+  </si>
+  <si>
+    <t>Modifier la génération et ajouter un dead end a l'intérieur du labyrinthe</t>
+  </si>
+  <si>
+    <t>J'avais sous estimmer cette fonctionalité lors de la plannifcation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de cette tache pour améliorer l'algorithme de recherche et le rendre plus pertinent </t>
   </si>
 </sst>
 </file>
@@ -970,7 +982,7 @@
   <dimension ref="A1:AM61"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G40" sqref="G40:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3658,16 +3670,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="108" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="15" max="15" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -3754,7 +3767,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="45"/>
       <c r="N3" s="50">
-        <f t="shared" ref="N3:N44" si="0">SUM(C3:M3)</f>
+        <f t="shared" ref="N3:N46" si="0">SUM(C3:M3)</f>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="P3" s="27" t="s">
@@ -3771,7 +3784,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="57">
-        <f t="shared" ref="B4:B54" si="1">SUM(C4:M4)</f>
+        <f t="shared" ref="B4:B56" si="1">SUM(C4:M4)</f>
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="C4" s="3"/>
@@ -4104,7 +4117,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>42</v>
       </c>
@@ -4130,7 +4143,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>27</v>
       </c>
@@ -4156,7 +4169,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>28</v>
       </c>
@@ -4182,7 +4195,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
         <v>60</v>
       </c>
@@ -4208,7 +4221,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>29</v>
       </c>
@@ -4234,7 +4247,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>30</v>
       </c>
@@ -4252,7 +4265,7 @@
       <c r="M22" s="40"/>
       <c r="N22" s="49"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>33</v>
       </c>
@@ -4274,11 +4287,11 @@
       <c r="L23" s="4"/>
       <c r="M23" s="43"/>
       <c r="N23" s="50">
-        <f t="shared" ref="N23:N36" si="3">SUM(C23:M23)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N23:N38" si="3">SUM(C23:M23)</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>46</v>
       </c>
@@ -4306,7 +4319,7 @@
         <v>0.12499999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>65</v>
       </c>
@@ -4334,7 +4347,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
         <v>61</v>
       </c>
@@ -4360,7 +4373,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
         <v>62</v>
       </c>
@@ -4386,7 +4399,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
         <v>63</v>
       </c>
@@ -4412,20 +4425,22 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="7"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -4433,23 +4448,25 @@
       <c r="M29" s="43"/>
       <c r="N29" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="B30" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
+      <c r="H30" s="20">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -4457,23 +4474,28 @@
       <c r="M30" s="43"/>
       <c r="N30" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>40</v>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="B31" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="H31" s="20">
+        <v>1.3888888888888888E-2</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -4481,23 +4503,28 @@
       <c r="M31" s="43"/>
       <c r="N31" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>48</v>
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="O31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
+        <v>44</v>
       </c>
       <c r="B32" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -4505,12 +4532,12 @@
       <c r="M32" s="43"/>
       <c r="N32" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B33" s="57">
         <f t="shared" si="1"/>
@@ -4521,7 +4548,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="7"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -4534,7 +4561,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B34" s="57">
         <f t="shared" si="1"/>
@@ -4545,7 +4572,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="7"/>
+      <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -4557,8 +4584,8 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
-        <v>31</v>
+      <c r="A35" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B35" s="57">
         <f t="shared" si="1"/>
@@ -4568,7 +4595,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="7"/>
+      <c r="G35" s="4"/>
       <c r="H35" s="7"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -4581,8 +4608,8 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
-        <v>32</v>
+      <c r="A36" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B36" s="57">
         <f t="shared" si="1"/>
@@ -4604,283 +4631,283 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="57">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="51"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="49"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="57">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="19">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="50">
-        <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="57">
-        <f t="shared" si="1"/>
-        <v>6.9444444444444434E-2</v>
-      </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="21">
-        <v>6.9444444444444434E-2</v>
-      </c>
-      <c r="H39" s="4"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="50">
-        <f t="shared" si="0"/>
-        <v>6.9444444444444434E-2</v>
-      </c>
+      <c r="B39" s="51"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="49"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="53" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B40" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" s="19">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="4"/>
       <c r="G40" s="5"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="46"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="45"/>
       <c r="N40" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="53" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B41" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="5"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="21">
+        <v>6.9444444444444434E-2</v>
+      </c>
       <c r="H41" s="4"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="46"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="45"/>
       <c r="N41" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="53" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B42" s="57">
         <f t="shared" si="1"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="20">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="F42" s="4"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="87"/>
-      <c r="K42" s="5"/>
+      <c r="H42" s="20">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="46"/>
       <c r="N42" s="50">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>39</v>
+      <c r="A43" s="53" t="s">
+        <v>37</v>
       </c>
       <c r="B43" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="4"/>
+      <c r="H43" s="20">
+        <v>2.7777777777777776E-2</v>
+      </c>
       <c r="I43" s="12"/>
-      <c r="J43" s="87"/>
+      <c r="J43" s="12"/>
       <c r="K43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="46"/>
       <c r="N43" s="50">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
-        <v>38</v>
+      <c r="A44" s="53" t="s">
+        <v>45</v>
       </c>
       <c r="B44" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
       <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="5"/>
       <c r="L44" s="12"/>
       <c r="M44" s="46"/>
       <c r="N44" s="50">
         <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="57">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="49"/>
-      <c r="Q45" s="25"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="53" t="s">
-        <v>8</v>
+      <c r="A46" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="B46" s="57">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C46" s="17">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D46" s="13"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="45"/>
+      <c r="H46" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="46"/>
       <c r="N46" s="50">
-        <f t="shared" ref="N46:N52" si="4">SUM(C46:M46)</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="53" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="57">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="C47" s="17">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="50">
-        <f t="shared" si="4"/>
-        <v>2.0833333333333332E-2</v>
-      </c>
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="51"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="49"/>
+      <c r="Q47" s="25"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B48" s="57">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C48" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D48" s="19">
-        <v>2.0833333333333332E-2</v>
-      </c>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D48" s="13"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -4891,13 +4918,13 @@
       <c r="L48" s="5"/>
       <c r="M48" s="45"/>
       <c r="N48" s="50">
-        <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <f t="shared" ref="N48:N54" si="4">SUM(C48:M48)</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="53" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B49" s="57">
         <f t="shared" si="1"/>
@@ -4923,234 +4950,292 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="53" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B50" s="57">
         <f t="shared" si="1"/>
-        <v>8.3333333333333343E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="C50" s="17">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D50" s="19">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E50" s="17">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="F50" s="19">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="G50" s="17">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="45"/>
       <c r="N50" s="50">
         <f t="shared" si="4"/>
-        <v>8.3333333333333343E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="55" t="s">
-        <v>3</v>
+      <c r="A51" s="53" t="s">
+        <v>10</v>
       </c>
       <c r="B51" s="57">
         <f t="shared" si="1"/>
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="C51" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D51" s="19">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="42"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="45"/>
       <c r="N51" s="50">
         <f t="shared" si="4"/>
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="55" t="s">
-        <v>4</v>
+      <c r="A52" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="B52" s="57">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="43"/>
+        <v>9.7222222222222238E-2</v>
+      </c>
+      <c r="C52" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D52" s="19">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E52" s="17">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="F52" s="19">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="G52" s="17">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H52" s="19">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
       <c r="N52" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9.7222222222222238E-2</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="55" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B53" s="57">
         <f t="shared" si="1"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C53" s="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C53" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D53" s="19">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="E53" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F53" s="19">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G53" s="17">
-        <v>4.1666666666666664E-2</v>
-      </c>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
+      <c r="M53" s="42"/>
       <c r="N53" s="50">
-        <f>SUM(C53:M53)</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="56" t="s">
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="55" t="s">
+        <v>4</v>
       </c>
       <c r="B54" s="57">
         <f t="shared" si="1"/>
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
-      <c r="E54" s="43"/>
-      <c r="F54" s="58">
-        <v>3.4722222222222224E-2</v>
-      </c>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43"/>
+        <v>0</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
       <c r="M54" s="43"/>
       <c r="N54" s="50">
-        <f>SUM(C54:M54)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="57">
+        <f t="shared" si="1"/>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E55" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F55" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G55" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="H55" s="19">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="50">
+        <f>SUM(C55:M55)</f>
+        <v>0.20833333333333331</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="57">
+        <f t="shared" si="1"/>
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="O54" t="s">
+      <c r="C56" s="43"/>
+      <c r="D56" s="43"/>
+      <c r="E56" s="43"/>
+      <c r="F56" s="58">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="G56" s="43"/>
+      <c r="H56" s="43"/>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="50">
+        <f>SUM(C56:M56)</f>
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="O56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
-      <c r="B55" s="62">
-        <f t="shared" ref="B55:M55" si="5">SUM(B2:B54)</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="C55" s="63">
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="10"/>
+      <c r="B57" s="62">
+        <f t="shared" ref="B57:M57" si="5">SUM(B2:B56)</f>
+        <v>1.9999999999999998</v>
+      </c>
+      <c r="C57" s="63">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D55" s="63">
+      <c r="D57" s="63">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E55" s="63">
+      <c r="E57" s="63">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F55" s="63">
+      <c r="F57" s="63">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G55" s="63">
+      <c r="G57" s="63">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H55" s="63">
+      <c r="H57" s="63">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="I57" s="63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I55" s="63">
+      <c r="J57" s="63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J55" s="63">
+      <c r="K57" s="63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K55" s="63">
+      <c r="L57" s="63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L55" s="63">
+      <c r="M57" s="63">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M55" s="63">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N55" s="64"/>
-      <c r="O55" s="65">
-        <f>SUM(N57-N56)</f>
+      <c r="N57" s="64"/>
+      <c r="O57" s="65">
+        <f>SUM(N59-N58)</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="K58" s="14"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="N58" s="52">
+        <f>SUM(N3:N57)</f>
         <v>1.9999999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="N56" s="52">
-        <f>SUM(N3:N55)</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N57" s="25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N59" s="25">
         <v>3.6666666666666665</v>
       </c>
     </row>

</xml_diff>